<commit_message>
add jasa to prk import
</commit_message>
<xml_diff>
--- a/public/templates/import_prk_template.xlsx
+++ b/public/templates/import_prk_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\monitoring-api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86458CE2-1DA8-48C2-B938-7D7C51CD588F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D23DD5E-37B2-4AAD-94E7-EEF8A64A885D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3B700C8B-DF7B-4FF2-AADC-B9758107657C}"/>
   </bookViews>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maul</author>
+    <author>Ichwan</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{B88B61BD-7719-4153-91A9-FEC5A64CB734}">
@@ -45,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{38A8F723-78FA-40AD-9693-66DA915331A4}">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{BC24E6F9-5A6D-4053-8F7B-E9F3F04005AB}">
       <text>
         <r>
           <rPr>
@@ -55,8 +56,38 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Wajib diisi
+          <t>Wajib diisi:
+MURNI
+LUNCURAN</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{38A8F723-78FA-40AD-9693-66DA915331A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Wajib diisi:
 Jika kosong, dianggap basket 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{6B337D7A-269A-4F66-AAE8-D642E2DEE77A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -65,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nama Project</t>
   </si>
@@ -92,6 +123,18 @@
   </si>
   <si>
     <t>2022.DDKI.5.002</t>
+  </si>
+  <si>
+    <t>Tipe</t>
+  </si>
+  <si>
+    <t>MURNI</t>
+  </si>
+  <si>
+    <t>LUNCURAN</t>
+  </si>
+  <si>
+    <t>RAB Jasa</t>
   </si>
 </sst>
 </file>
@@ -100,7 +143,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -165,12 +208,15 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -490,18 +536,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0055F1BE-D36D-4900-BAE7-AAE317A6DB22}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,10 +563,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -531,11 +585,17 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
         <v>3</v>
       </c>
+      <c r="G2" s="3">
+        <v>90000000</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -548,8 +608,14 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
         <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>100000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>